<commit_message>
Print Orders summary completed
</commit_message>
<xml_diff>
--- a/LogAnalyzer/ReportPattern/LogAnalysis.xlsx
+++ b/LogAnalyzer/ReportPattern/LogAnalysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Виктор\source\repos\CourierLogisticsEx\LogAnalyzer\ReportPattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BADC8B4-3810-476A-B90B-33D80A692A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13B546A-F9D4-45EF-80D2-FBCB117F0BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="348" windowWidth="22968" windowHeight="11196" tabRatio="685" activeTab="7" xr2:uid="{953046DB-BB6E-45BE-A634-FFA4A2A614DD}"/>
+    <workbookView xWindow="768" yWindow="636" windowWidth="22968" windowHeight="11196" tabRatio="685" activeTab="3" xr2:uid="{953046DB-BB6E-45BE-A634-FFA4A2A614DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="7" r:id="rId1"/>
     <sheet name="Orders Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="Errors Summary" sheetId="2" r:id="rId3"/>
+    <sheet name="Error summary" sheetId="12" r:id="rId3"/>
     <sheet name="Order Events" sheetId="3" r:id="rId4"/>
     <sheet name="Shop Events" sheetId="8" r:id="rId5"/>
     <sheet name="Courier Events" sheetId="9" r:id="rId6"/>
@@ -26,6 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Cancel Commands'!$A$2:$AA$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Courier Events'!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Delivery Commands'!$A$2:$BD$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Error summary'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Order Events'!$A$1:$V$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Orders Summary'!$A$2:$AQ$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Shop Events'!$A$1:$I$1</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
   <si>
     <t>order_id</t>
   </si>
@@ -613,6 +614,21 @@
   </si>
   <si>
     <t>5 - Gett-такси.</t>
+  </si>
+  <si>
+    <t>date_time</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>rc</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>call args</t>
   </si>
 </sst>
 </file>
@@ -750,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -965,11 +981,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1025,6 +1086,63 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1058,70 +1176,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1130,8 +1194,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1683,90 +1759,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="39" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="42" t="s">
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="48" t="s">
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="62"/>
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="45" t="s">
+      <c r="AL1" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="47"/>
-      <c r="AO1" s="45" t="s">
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="47"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="66"/>
     </row>
     <row r="2" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="51"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="24" t="s">
         <v>6</v>
       </c>
@@ -1848,7 +1924,7 @@
       <c r="AJ2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="49"/>
+      <c r="AK2" s="68"/>
       <c r="AL2" s="35" t="s">
         <v>18</v>
       </c>
@@ -1871,6 +1947,11 @@
   </sheetData>
   <autoFilter ref="A2:AQ2" xr:uid="{358CE2C5-DC6A-4F55-A9CA-4BBC233098CA}"/>
   <mergeCells count="15">
+    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="A1:A2"/>
@@ -1881,11 +1962,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="S1:AA1"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AK1:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1893,15 +1969,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928BF863-688B-44B4-83EA-EBAD553D21F5}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDDCBD5-80D3-4E0E-97C1-5818588A00FB}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" customWidth="1"/>
+    <col min="6" max="6" width="83.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{342EF910-3C73-4F17-AEBD-F6EA27697742}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1910,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC439B5-413A-438C-B229-359F9B74470C}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
@@ -2185,7 +2289,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="69" t="s">
@@ -2239,55 +2343,55 @@
       <c r="R1" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="70" t="s">
+      <c r="S1" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="T1" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="45" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="47"/>
-      <c r="AM1" s="45" t="s">
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="47"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="65"/>
+      <c r="AX1" s="65"/>
+      <c r="AY1" s="65"/>
+      <c r="AZ1" s="65"/>
+      <c r="BA1" s="65"/>
+      <c r="BB1" s="65"/>
+      <c r="BC1" s="65"/>
+      <c r="BD1" s="66"/>
     </row>
     <row r="2" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="71"/>
+      <c r="A2" s="70"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
@@ -2305,7 +2409,7 @@
       <c r="P2" s="69"/>
       <c r="Q2" s="69"/>
       <c r="R2" s="69"/>
-      <c r="S2" s="70"/>
+      <c r="S2" s="71"/>
       <c r="T2" s="15" t="s">
         <v>74</v>
       </c>
@@ -2436,14 +2540,6 @@
   </sheetData>
   <autoFilter ref="A2:BD2" xr:uid="{83EE47D8-74F9-4A4F-B86A-3C3FF7BC8616}"/>
   <mergeCells count="22">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="AM1:BD1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -2458,6 +2554,14 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2468,7 +2572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4335C45C-9BDC-4EC3-ADBA-63318EACD2BD}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
@@ -2484,81 +2588,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="45" t="s">
+      <c r="N1" s="65"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="45" t="s">
+      <c r="Q1" s="65"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="T1" s="46"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="45" t="s">
+      <c r="T1" s="65"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="W1" s="46"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="45" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="47"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="66"/>
     </row>
     <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="74"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="73"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="74"/>
       <c r="M2" s="15" t="s">
         <v>5</v>
       </c>
@@ -2614,11 +2718,7 @@
   </sheetData>
   <autoFilter ref="A2:AA2" xr:uid="{95B6FF3A-736D-4F88-A268-A923A9F80D4E}"/>
   <mergeCells count="17">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="H1:H2"/>
@@ -2626,11 +2726,15 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:X1"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create all report pages
</commit_message>
<xml_diff>
--- a/LogAnalyzer/ReportPattern/LogAnalysis.xlsx
+++ b/LogAnalyzer/ReportPattern/LogAnalysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Виктор\source\repos\CourierLogisticsEx\LogAnalyzer\ReportPattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13B546A-F9D4-45EF-80D2-FBCB117F0BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93CD785-E438-4E09-B689-67BA03B3AC7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="636" windowWidth="22968" windowHeight="11196" tabRatio="685" activeTab="3" xr2:uid="{953046DB-BB6E-45BE-A634-FFA4A2A614DD}"/>
+    <workbookView xWindow="108" yWindow="1416" windowWidth="22968" windowHeight="11196" tabRatio="685" activeTab="7" xr2:uid="{953046DB-BB6E-45BE-A634-FFA4A2A614DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="7" r:id="rId1"/>
     <sheet name="Orders Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="Error summary" sheetId="12" r:id="rId3"/>
+    <sheet name="Error summary" sheetId="13" r:id="rId3"/>
     <sheet name="Order Events" sheetId="3" r:id="rId4"/>
     <sheet name="Shop Events" sheetId="8" r:id="rId5"/>
     <sheet name="Courier Events" sheetId="9" r:id="rId6"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="136">
   <si>
     <t>order_id</t>
   </si>
@@ -415,9 +415,6 @@
     <t>courier_type</t>
   </si>
   <si>
-    <t>walking</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -628,7 +625,7 @@
     <t>message</t>
   </si>
   <si>
-    <t>call args</t>
+    <t>msg_no</t>
   </si>
 </sst>
 </file>
@@ -766,7 +763,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1011,26 +1008,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1047,7 +1029,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1069,23 +1050,62 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1143,71 +1163,55 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1628,85 +1632,85 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="31"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1721,7 +1725,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="V1" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="AM13" sqref="AM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,223 +1739,218 @@
     <col min="7" max="7" width="2.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="2.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="6.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.77734375" style="4" customWidth="1"/>
+    <col min="10" max="11" width="15.77734375" style="76" customWidth="1"/>
     <col min="12" max="12" width="4.88671875" style="4" customWidth="1"/>
-    <col min="13" max="14" width="15.77734375" style="4" customWidth="1"/>
+    <col min="13" max="14" width="15.77734375" style="76" customWidth="1"/>
     <col min="15" max="15" width="8.44140625" style="4" customWidth="1"/>
     <col min="16" max="16" width="4.44140625" style="4" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.77734375" style="3" customWidth="1"/>
+    <col min="19" max="20" width="15.77734375" style="80" customWidth="1"/>
     <col min="21" max="21" width="4.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.77734375" style="3" customWidth="1"/>
+    <col min="22" max="23" width="15.77734375" style="80" customWidth="1"/>
     <col min="24" max="24" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="27" width="4.44140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="15.77734375" style="2" customWidth="1"/>
-    <col min="29" max="29" width="15.88671875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="15.77734375" style="83" customWidth="1"/>
+    <col min="29" max="29" width="15.88671875" style="83" customWidth="1"/>
     <col min="30" max="30" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="15.77734375" style="2" customWidth="1"/>
+    <col min="31" max="32" width="15.77734375" style="83" customWidth="1"/>
     <col min="33" max="33" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="34" max="36" width="4.44140625" style="2" customWidth="1"/>
     <col min="37" max="37" width="5.33203125" customWidth="1"/>
-    <col min="38" max="38" width="15.77734375" customWidth="1"/>
-    <col min="41" max="41" width="15.77734375" customWidth="1"/>
+    <col min="38" max="38" width="15.77734375" style="11" customWidth="1"/>
+    <col min="41" max="41" width="15.77734375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="58" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="61" t="s">
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="67" t="s">
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="64" t="s">
+      <c r="AL1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="64" t="s">
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="66"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="46"/>
     </row>
     <row r="2" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="24" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="S2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="X2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="Y2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="28" t="s">
+      <c r="Z2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="30" t="s">
+      <c r="AB2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AC2" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="31" t="s">
+      <c r="AD2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="31" t="s">
+      <c r="AE2" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="31" t="s">
+      <c r="AF2" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="31" t="s">
+      <c r="AG2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AH2" s="31" t="s">
+      <c r="AH2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="31" t="s">
+      <c r="AI2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AJ2" s="32" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="68"/>
-      <c r="AL2" s="35" t="s">
+      <c r="AK2" s="48"/>
+      <c r="AL2" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="AM2" s="33" t="s">
+      <c r="AM2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="AN2" s="34" t="s">
+      <c r="AN2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="35" t="s">
+      <c r="AO2" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="AP2" s="33" t="s">
+      <c r="AP2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="AQ2" s="34" t="s">
+      <c r="AQ2" s="30" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:AQ2" xr:uid="{358CE2C5-DC6A-4F55-A9CA-4BBC233098CA}"/>
   <mergeCells count="15">
-    <mergeCell ref="S1:AA1"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="A1:A2"/>
@@ -1962,6 +1961,11 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AK1:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1969,39 +1973,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDDCBD5-80D3-4E0E-97C1-5818588A00FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCE7923-BB3A-4ED5-AF9E-0536B9E29C3A}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="66.6640625" customWidth="1"/>
-    <col min="6" max="6" width="83.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="E1" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="F1" s="37" t="s">
         <v>134</v>
-      </c>
-      <c r="E1" s="78" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="79" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2012,23 +2017,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC439B5-413A-438C-B229-359F9B74470C}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.77734375" customWidth="1"/>
+    <col min="9" max="10" width="15.77734375" style="11" customWidth="1"/>
     <col min="11" max="14" width="10.109375" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" customWidth="1"/>
     <col min="22" max="22" width="8.88671875" customWidth="1"/>
@@ -2038,7 +2043,7 @@
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="85" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -2047,7 +2052,7 @@
       <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="85" t="s">
         <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -2059,10 +2064,10 @@
       <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="85" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="10" t="s">
@@ -2100,16 +2105,6 @@
       </c>
       <c r="V1" s="10" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="E2" s="11">
-        <v>44164.433159722219</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2">
-        <v>35.123455999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2120,20 +2115,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3229C91-947D-4FF8-B03C-46CEF5F941A5}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15.77734375" customWidth="1"/>
+    <col min="5" max="7" width="15.77734375" style="11" customWidth="1"/>
     <col min="8" max="9" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2141,7 +2136,7 @@
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="85" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -2150,13 +2145,13 @@
       <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="85" t="s">
         <v>62</v>
       </c>
       <c r="H1" s="10" t="s">
@@ -2164,16 +2159,6 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E2" s="11">
-        <v>44164.433159722219</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2">
-        <v>35.123455999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2184,23 +2169,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D573740-B630-4AFE-8B61-545D01BE7C95}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.77734375" customWidth="1"/>
+    <col min="9" max="10" width="15.77734375" style="11" customWidth="1"/>
     <col min="11" max="12" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2208,7 +2193,7 @@
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="85" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="10" t="s">
@@ -2217,7 +2202,7 @@
       <c r="D1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="85" t="s">
         <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -2229,30 +2214,17 @@
       <c r="H1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="85" t="s">
         <v>62</v>
       </c>
       <c r="K1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E2" s="11">
-        <v>44164.433159722219</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2">
-        <v>35.123455999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2267,279 +2239,276 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" customWidth="1"/>
-    <col min="8" max="10" width="15.77734375" customWidth="1"/>
+    <col min="8" max="10" width="15.77734375" style="11" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.77734375" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.77734375" style="11" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="89" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.21875" customWidth="1"/>
     <col min="19" max="19" width="13.109375" customWidth="1"/>
-    <col min="20" max="28" width="6.21875" style="13" customWidth="1"/>
-    <col min="29" max="38" width="5.5546875" style="13" customWidth="1"/>
-    <col min="39" max="56" width="7.77734375" style="13" customWidth="1"/>
+    <col min="20" max="28" width="6.21875" style="12" customWidth="1"/>
+    <col min="29" max="38" width="5.5546875" style="12" customWidth="1"/>
+    <col min="39" max="56" width="7.77734375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="69" t="s">
+      <c r="G1" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="69" t="s">
+      <c r="I1" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="L1" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="M1" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="69" t="s">
+      <c r="N1" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="69" t="s">
+      <c r="O1" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="69" t="s">
+      <c r="P1" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="Q1" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="69" t="s">
+      <c r="R1" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="R1" s="69" t="s">
+      <c r="S1" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="T1" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="T1" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="64" t="s">
-        <v>107</v>
-      </c>
-      <c r="AN1" s="65"/>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="65"/>
-      <c r="AS1" s="65"/>
-      <c r="AT1" s="65"/>
-      <c r="AU1" s="65"/>
-      <c r="AV1" s="65"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="65"/>
-      <c r="AY1" s="65"/>
-      <c r="AZ1" s="65"/>
-      <c r="BA1" s="65"/>
-      <c r="BB1" s="65"/>
-      <c r="BC1" s="65"/>
-      <c r="BD1" s="66"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AX1" s="45"/>
+      <c r="AY1" s="45"/>
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="46"/>
     </row>
     <row r="2" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="70"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="U2" s="16">
+      <c r="B2" s="86"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="15">
         <v>1</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="15">
         <v>2</v>
       </c>
-      <c r="W2" s="16">
+      <c r="W2" s="15">
         <v>3</v>
       </c>
-      <c r="X2" s="16">
+      <c r="X2" s="15">
         <v>4</v>
       </c>
-      <c r="Y2" s="16">
+      <c r="Y2" s="15">
         <v>5</v>
       </c>
-      <c r="Z2" s="16">
+      <c r="Z2" s="15">
         <v>6</v>
       </c>
-      <c r="AA2" s="16">
+      <c r="AA2" s="15">
         <v>7</v>
       </c>
-      <c r="AB2" s="17">
+      <c r="AB2" s="16">
         <v>8</v>
       </c>
-      <c r="AC2" s="20" t="s">
+      <c r="AC2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE2" s="21">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="21">
+        <v>3</v>
+      </c>
+      <c r="AG2" s="21">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="21">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="21">
+        <v>6</v>
+      </c>
+      <c r="AJ2" s="21">
+        <v>7</v>
+      </c>
+      <c r="AK2" s="21">
+        <v>8</v>
+      </c>
+      <c r="AL2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="AD2" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE2" s="22">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="22">
-        <v>3</v>
-      </c>
-      <c r="AG2" s="22">
-        <v>4</v>
-      </c>
-      <c r="AH2" s="22">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="22">
-        <v>6</v>
-      </c>
-      <c r="AJ2" s="22">
-        <v>7</v>
-      </c>
-      <c r="AK2" s="22">
-        <v>8</v>
-      </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AM2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AN2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="AN2" s="18" t="s">
+      <c r="AO2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="AO2" s="18" t="s">
+      <c r="AP2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AQ2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AQ2" s="18" t="s">
+      <c r="AR2" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AS2" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="AS2" s="18" t="s">
+      <c r="AT2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="AT2" s="18" t="s">
+      <c r="AU2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="AU2" s="18" t="s">
+      <c r="AV2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AW2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="AW2" s="18" t="s">
+      <c r="AX2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="AX2" s="18" t="s">
+      <c r="AY2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="AY2" s="18" t="s">
+      <c r="AZ2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="AZ2" s="18" t="s">
+      <c r="BA2" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="BA2" s="18" t="s">
+      <c r="BB2" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="BB2" s="18" t="s">
+      <c r="BC2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="BC2" s="18" t="s">
+      <c r="BD2" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="BD2" s="19" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="J3" s="12"/>
-      <c r="U3" s="13">
-        <v>9372767</v>
-      </c>
-      <c r="AD3" s="14">
-        <v>5.8067129629629628E-2</v>
-      </c>
-      <c r="AM3" s="13">
-        <v>10237</v>
-      </c>
-      <c r="AN3" s="13">
-        <v>10000</v>
-      </c>
+      <c r="J3" s="87"/>
+      <c r="AD3" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:BD2" xr:uid="{83EE47D8-74F9-4A4F-B86A-3C3FF7BC8616}"/>
   <mergeCells count="22">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="AM1:BD1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -2554,14 +2523,6 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2572,152 +2533,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4335C45C-9BDC-4EC3-ADBA-63318EACD2BD}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
     <col min="4" max="5" width="7.88671875" customWidth="1"/>
-    <col min="9" max="11" width="15.77734375" customWidth="1"/>
+    <col min="9" max="11" width="15.77734375" style="11" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="6.21875" style="13" customWidth="1"/>
+    <col min="13" max="15" width="6.21875" style="12" customWidth="1"/>
     <col min="16" max="27" width="6.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="46" t="s">
+      <c r="J1" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="73" t="s">
+      <c r="K1" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" s="45"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="45"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="W1" s="45"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="46"/>
+    </row>
+    <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="73"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="64" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="W1" s="65"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="66"/>
-    </row>
-    <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="72"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="15" t="s">
+      <c r="P2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="O2" s="23" t="s">
+      <c r="Q2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="R2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="R2" s="23" t="s">
+      <c r="T2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="U2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="V2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="U2" s="23" t="s">
+      <c r="W2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="X2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="X2" s="23" t="s">
+      <c r="Z2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="Y2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA2" s="23" t="s">
-        <v>110</v>
+      <c r="AA2" s="22" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="K3" s="12"/>
-      <c r="N3" s="13">
-        <v>9372767</v>
-      </c>
+      <c r="K3" s="87"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA2" xr:uid="{95B6FF3A-736D-4F88-A268-A923A9F80D4E}"/>
   <mergeCells count="17">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="L1:L2"/>
@@ -2729,12 +2693,6 @@
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:X1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Log Analyzer debug is completed
</commit_message>
<xml_diff>
--- a/LogAnalyzer/ReportPattern/LogAnalysis.xlsx
+++ b/LogAnalyzer/ReportPattern/LogAnalysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Виктор\source\repos\CourierLogisticsEx\LogAnalyzer\ReportPattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93CD785-E438-4E09-B689-67BA03B3AC7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C66998F-0976-4698-9958-C3CFDF031B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="1416" windowWidth="22968" windowHeight="11196" tabRatio="685" activeTab="7" xr2:uid="{953046DB-BB6E-45BE-A634-FFA4A2A614DD}"/>
+    <workbookView xWindow="72" yWindow="384" windowWidth="22968" windowHeight="11196" tabRatio="685" activeTab="6" xr2:uid="{953046DB-BB6E-45BE-A634-FFA4A2A614DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="7" r:id="rId1"/>
     <sheet name="Orders Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="Error summary" sheetId="13" r:id="rId3"/>
+    <sheet name="Errors summary" sheetId="13" r:id="rId3"/>
     <sheet name="Order Events" sheetId="3" r:id="rId4"/>
     <sheet name="Shop Events" sheetId="8" r:id="rId5"/>
     <sheet name="Courier Events" sheetId="9" r:id="rId6"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Cancel Commands'!$A$2:$AA$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Courier Events'!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Delivery Commands'!$A$2:$BD$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Error summary'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Errors summary'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Order Events'!$A$1:$V$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Orders Summary'!$A$2:$AQ$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Shop Events'!$A$1:$I$1</definedName>
@@ -1012,14 +1012,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1029,33 +1026,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="21" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1072,114 +1045,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1199,18 +1064,184 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1546,7 +1577,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1591,7 +1622,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
@@ -1623,7 +1654,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
@@ -1631,85 +1662,85 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="15" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="15" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="15" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
+      <c r="A22" s="14"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="16" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="15" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="15" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="15" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="15" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="15" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="15" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1725,232 +1756,237 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="V1" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="AM13" sqref="AM13"/>
+      <selection pane="bottomLeft" activeCell="AH2" sqref="AH1:AJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="35" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="2.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.77734375" style="76" customWidth="1"/>
-    <col min="12" max="12" width="4.88671875" style="4" customWidth="1"/>
-    <col min="13" max="14" width="15.77734375" style="76" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="4.44140625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.77734375" style="80" customWidth="1"/>
-    <col min="21" max="21" width="4.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.77734375" style="80" customWidth="1"/>
-    <col min="24" max="24" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="4.44140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="15.77734375" style="83" customWidth="1"/>
-    <col min="29" max="29" width="15.88671875" style="83" customWidth="1"/>
-    <col min="30" max="30" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="15.77734375" style="83" customWidth="1"/>
-    <col min="33" max="33" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="4.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.33203125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="2.33203125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.77734375" style="23" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" style="3" customWidth="1"/>
+    <col min="13" max="14" width="15.77734375" style="23" customWidth="1"/>
+    <col min="15" max="15" width="8.44140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="4.44140625" style="43" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.77734375" style="27" customWidth="1"/>
+    <col min="21" max="21" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="15.77734375" style="27" customWidth="1"/>
+    <col min="24" max="24" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="4.44140625" style="37" customWidth="1"/>
+    <col min="28" max="28" width="15.77734375" style="30" customWidth="1"/>
+    <col min="29" max="29" width="15.88671875" style="30" customWidth="1"/>
+    <col min="30" max="30" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.77734375" style="30" customWidth="1"/>
+    <col min="33" max="33" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="4.44140625" style="39" customWidth="1"/>
     <col min="37" max="37" width="5.33203125" customWidth="1"/>
-    <col min="38" max="38" width="15.77734375" style="11" customWidth="1"/>
-    <col min="41" max="41" width="15.77734375" style="11" customWidth="1"/>
+    <col min="38" max="38" width="15.77734375" style="8" customWidth="1"/>
+    <col min="41" max="41" width="15.77734375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="38" t="s">
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="41" t="s">
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AI1" s="42"/>
-      <c r="AJ1" s="43"/>
-      <c r="AK1" s="47" t="s">
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="84"/>
+      <c r="AI1" s="84"/>
+      <c r="AJ1" s="85"/>
+      <c r="AK1" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="44" t="s">
+      <c r="AL1" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="44" t="s">
+      <c r="AM1" s="87"/>
+      <c r="AN1" s="88"/>
+      <c r="AO1" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="46"/>
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="88"/>
     </row>
     <row r="2" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="75" t="s">
+      <c r="A2" s="65"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="77" t="s">
+      <c r="K2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="77" t="s">
+      <c r="M2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="77" t="s">
+      <c r="N2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="Q2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="78" t="s">
+      <c r="S2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="79" t="s">
+      <c r="T2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="25" t="s">
+      <c r="U2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="79" t="s">
+      <c r="V2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="79" t="s">
+      <c r="W2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="26" t="s">
+      <c r="AA2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="81" t="s">
+      <c r="AB2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="82" t="s">
+      <c r="AC2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="27" t="s">
+      <c r="AD2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="82" t="s">
+      <c r="AE2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="82" t="s">
+      <c r="AF2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AH2" s="27" t="s">
+      <c r="AH2" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="27" t="s">
+      <c r="AI2" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="84" t="s">
+      <c r="AK2" s="90"/>
+      <c r="AL2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AM2" s="29" t="s">
+      <c r="AM2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AN2" s="30" t="s">
+      <c r="AN2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="84" t="s">
+      <c r="AO2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AP2" s="29" t="s">
+      <c r="AP2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AQ2" s="30" t="s">
+      <c r="AQ2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:AQ2" xr:uid="{358CE2C5-DC6A-4F55-A9CA-4BBC233098CA}"/>
   <mergeCells count="15">
+    <mergeCell ref="S1:AA1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="A1:A2"/>
@@ -1961,11 +1997,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="S1:AA1"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AK1:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1978,34 +2009,34 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="8" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
     <col min="6" max="6" width="121.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2026,84 +2057,84 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="8" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.77734375" style="11" customWidth="1"/>
+    <col min="9" max="10" width="15.77734375" style="8" customWidth="1"/>
     <col min="11" max="14" width="10.109375" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" customWidth="1"/>
     <col min="22" max="22" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="85" t="s">
+      <c r="I1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2125,39 +2156,39 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="8" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15.77734375" style="11" customWidth="1"/>
+    <col min="5" max="7" width="15.77734375" style="8" customWidth="1"/>
     <col min="8" max="9" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="G1" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2178,52 +2209,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="8" customWidth="1"/>
     <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.77734375" style="11" customWidth="1"/>
+    <col min="9" max="10" width="15.77734375" style="8" customWidth="1"/>
     <col min="11" max="12" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="85" t="s">
+      <c r="I1" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2237,278 +2268,270 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1660D130-0909-42C6-A5CD-673621A16207}">
   <dimension ref="A1:BD3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="8" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" customWidth="1"/>
-    <col min="8" max="10" width="15.77734375" style="11" customWidth="1"/>
+    <col min="8" max="10" width="15.77734375" style="8" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.77734375" style="11" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="89" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.77734375" style="8" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="34" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.21875" customWidth="1"/>
     <col min="19" max="19" width="13.109375" customWidth="1"/>
-    <col min="20" max="28" width="6.21875" style="12" customWidth="1"/>
-    <col min="29" max="38" width="5.5546875" style="12" customWidth="1"/>
-    <col min="39" max="56" width="7.77734375" style="12" customWidth="1"/>
+    <col min="20" max="20" width="6.21875" style="51" customWidth="1"/>
+    <col min="21" max="28" width="7" style="51" customWidth="1"/>
+    <col min="29" max="38" width="5.5546875" style="55" customWidth="1"/>
+    <col min="39" max="56" width="7.77734375" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:56" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="91" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="M1" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="68" t="s">
+      <c r="N1" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="86" t="s">
+      <c r="O1" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="86" t="s">
+      <c r="P1" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="88" t="s">
+      <c r="Q1" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="S1" s="69" t="s">
+      <c r="S1" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="44" t="s">
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="96"/>
+      <c r="AC1" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
-      <c r="AK1" s="45"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="44" t="s">
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="98"/>
+      <c r="AG1" s="98"/>
+      <c r="AH1" s="98"/>
+      <c r="AI1" s="98"/>
+      <c r="AJ1" s="98"/>
+      <c r="AK1" s="98"/>
+      <c r="AL1" s="99"/>
+      <c r="AM1" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="AN1" s="45"/>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="45"/>
-      <c r="AR1" s="45"/>
-      <c r="AS1" s="45"/>
-      <c r="AT1" s="45"/>
-      <c r="AU1" s="45"/>
-      <c r="AV1" s="45"/>
-      <c r="AW1" s="45"/>
-      <c r="AX1" s="45"/>
-      <c r="AY1" s="45"/>
-      <c r="AZ1" s="45"/>
-      <c r="BA1" s="45"/>
-      <c r="BB1" s="45"/>
-      <c r="BC1" s="45"/>
-      <c r="BD1" s="46"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="95"/>
+      <c r="AP1" s="95"/>
+      <c r="AQ1" s="95"/>
+      <c r="AR1" s="95"/>
+      <c r="AS1" s="95"/>
+      <c r="AT1" s="95"/>
+      <c r="AU1" s="95"/>
+      <c r="AV1" s="95"/>
+      <c r="AW1" s="95"/>
+      <c r="AX1" s="95"/>
+      <c r="AY1" s="95"/>
+      <c r="AZ1" s="95"/>
+      <c r="BA1" s="95"/>
+      <c r="BB1" s="95"/>
+      <c r="BC1" s="95"/>
+      <c r="BD1" s="96"/>
     </row>
     <row r="2" spans="1:56" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="70"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="14" t="s">
+      <c r="A2" s="93"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="U2" s="15">
+      <c r="U2" s="49">
         <v>1</v>
       </c>
-      <c r="V2" s="15">
+      <c r="V2" s="49">
         <v>2</v>
       </c>
-      <c r="W2" s="15">
+      <c r="W2" s="49">
         <v>3</v>
       </c>
-      <c r="X2" s="15">
+      <c r="X2" s="49">
         <v>4</v>
       </c>
-      <c r="Y2" s="15">
+      <c r="Y2" s="49">
         <v>5</v>
       </c>
-      <c r="Z2" s="15">
+      <c r="Z2" s="49">
         <v>6</v>
       </c>
-      <c r="AA2" s="15">
+      <c r="AA2" s="49">
         <v>7</v>
       </c>
-      <c r="AB2" s="16">
+      <c r="AB2" s="50">
         <v>8</v>
       </c>
-      <c r="AC2" s="19" t="s">
+      <c r="AC2" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="AD2" s="21" t="s">
+      <c r="AD2" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="AE2" s="21">
+      <c r="AE2" s="53">
         <v>2</v>
       </c>
-      <c r="AF2" s="21">
+      <c r="AF2" s="53">
         <v>3</v>
       </c>
-      <c r="AG2" s="21">
+      <c r="AG2" s="53">
         <v>4</v>
       </c>
-      <c r="AH2" s="21">
+      <c r="AH2" s="53">
         <v>5</v>
       </c>
-      <c r="AI2" s="21">
+      <c r="AI2" s="53">
         <v>6</v>
       </c>
-      <c r="AJ2" s="21">
+      <c r="AJ2" s="53">
         <v>7</v>
       </c>
-      <c r="AK2" s="21">
+      <c r="AK2" s="53">
         <v>8</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AL2" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="AN2" s="17" t="s">
+      <c r="AN2" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="AO2" s="17" t="s">
+      <c r="AO2" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="AP2" s="17" t="s">
+      <c r="AP2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="AQ2" s="17" t="s">
+      <c r="AQ2" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="AR2" s="17" t="s">
+      <c r="AR2" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="AS2" s="17" t="s">
+      <c r="AS2" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="AT2" s="17" t="s">
+      <c r="AT2" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="AU2" s="17" t="s">
+      <c r="AU2" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="AV2" s="17" t="s">
+      <c r="AV2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="AW2" s="17" t="s">
+      <c r="AW2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="AX2" s="17" t="s">
+      <c r="AX2" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="AY2" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="AZ2" s="17" t="s">
+      <c r="AZ2" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="BA2" s="17" t="s">
+      <c r="BA2" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="BB2" s="17" t="s">
+      <c r="BB2" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="BC2" s="17" t="s">
+      <c r="BC2" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="BD2" s="18" t="s">
+      <c r="BD2" s="57" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="J3" s="87"/>
-      <c r="AD3" s="13"/>
+      <c r="J3" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:BD2" xr:uid="{83EE47D8-74F9-4A4F-B86A-3C3FF7BC8616}"/>
   <mergeCells count="22">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="AM1:BD1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
@@ -2523,6 +2546,14 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2533,155 +2564,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4335C45C-9BDC-4EC3-ADBA-63318EACD2BD}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="8" customWidth="1"/>
     <col min="4" max="5" width="7.88671875" customWidth="1"/>
-    <col min="9" max="11" width="15.77734375" style="11" customWidth="1"/>
+    <col min="9" max="11" width="15.77734375" style="8" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="6.21875" style="12" customWidth="1"/>
-    <col min="16" max="27" width="6.21875" customWidth="1"/>
+    <col min="13" max="15" width="6.21875" style="51" customWidth="1"/>
+    <col min="16" max="27" width="6.21875" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="103" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="44" t="s">
+      <c r="N1" s="95"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="44" t="s">
+      <c r="Q1" s="95"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="45"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="44" t="s">
+      <c r="T1" s="95"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="W1" s="45"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="44" t="s">
+      <c r="W1" s="95"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="46"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="96"/>
     </row>
     <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="14" t="s">
+      <c r="A2" s="102"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="R2" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="U2" s="22" t="s">
+      <c r="U2" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="X2" s="22" t="s">
+      <c r="X2" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="AA2" s="22" t="s">
+      <c r="AA2" s="58" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="K3" s="87"/>
+      <c r="K3" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA2" xr:uid="{95B6FF3A-736D-4F88-A268-A923A9F80D4E}"/>
   <mergeCells count="17">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="L1:L2"/>
@@ -2693,6 +2718,12 @@
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:X1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>